<commit_message>
updated filter function for empty assigned staff, CAPEX & OPEX and Link
</commit_message>
<xml_diff>
--- a/Excel File 1.xlsx
+++ b/Excel File 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C31AC1-A402-418C-AF59-1B53D4BAFF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28416F2B-66DC-42D3-A43C-CB69D558F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>PJR2022210</t>
   </si>
   <si>
-    <t>Chee Ching</t>
-  </si>
-  <si>
     <t>3/18/2022 11:02</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>SOWVA</t>
+  </si>
+  <si>
+    <t>aik wei</t>
   </si>
 </sst>
 </file>
@@ -150,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +436,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,49 +459,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -517,16 +518,16 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -547,27 +548,30 @@
         <v>22</v>
       </c>
       <c r="O2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
+      <c r="G3" s="1">
+        <v>45509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>